<commit_message>
build + sim + adc fix
</commit_message>
<xml_diff>
--- a/simulation/results/simSet9Results/simSet9.xlsx
+++ b/simulation/results/simSet9Results/simSet9.xlsx
@@ -852,6 +852,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -882,6 +885,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -906,6 +912,99 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
+  <twoCellAnchor editAs="twoCell">
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>9</row>
+      <rowOff>0</rowOff>
+    </from>
+    <to>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>10</row>
+      <rowOff>0</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="25" name="Image 25" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
+  <twoCellAnchor editAs="twoCell">
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>9</row>
+      <rowOff>0</rowOff>
+    </from>
+    <to>
+      <col>11</col>
+      <colOff>0</colOff>
+      <row>10</row>
+      <rowOff>0</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="26" name="Image 26" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
+  <twoCellAnchor editAs="twoCell">
+    <from>
+      <col>11</col>
+      <colOff>0</colOff>
+      <row>9</row>
+      <rowOff>0</rowOff>
+    </from>
+    <to>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>10</row>
+      <rowOff>0</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="27" name="Image 27" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId27"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1208,7 +1307,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1220,7 +1319,7 @@
     <col width="16" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="13" customWidth="1" min="5" max="5"/>
-    <col width="70" customWidth="1" min="10" max="10"/>
+    <col width="55" customWidth="1" min="10" max="10"/>
     <col width="50" customWidth="1" min="11" max="11"/>
     <col width="70" customWidth="1" min="12" max="12"/>
   </cols>
@@ -1461,16 +1560,16 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>200</v>
+        <v>47</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>2.7</v>
@@ -1489,21 +1588,49 @@
         <v>2</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>294</v>
+        <v>100</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>2.7</v>
       </c>
       <c r="H9" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" ht="240" customHeight="1">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="H10" s="2" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>